<commit_message>
Update LLM for Engineers - 64 hrs -Updated Day wise Schedule V2.0 5 OCT.xlsx
</commit_message>
<xml_diff>
--- a/LLM for Engineers - 64 hrs -Updated Day wise Schedule V2.0 5 OCT.xlsx
+++ b/LLM for Engineers - 64 hrs -Updated Day wise Schedule V2.0 5 OCT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gridflowAI\NIIT-Tredence-LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AFA860-C5D3-488F-885F-BDD705239799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A38BA9A-B77C-48CE-98DD-9450010EAE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="-8700" windowWidth="17910" windowHeight="14550" activeTab="1" xr2:uid="{A8A0E829-4FD1-4464-B06B-3E7B94940585}"/>
+    <workbookView xWindow="38520" yWindow="-8685" windowWidth="18660" windowHeight="13830" xr2:uid="{A8A0E829-4FD1-4464-B06B-3E7B94940585}"/>
   </bookViews>
   <sheets>
     <sheet name="Updated Schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="194">
   <si>
     <t>Phase</t>
   </si>
@@ -666,12 +666,18 @@
   <si>
     <t>DEMO : BM25</t>
   </si>
+  <si>
+    <t>18th dec</t>
+  </si>
+  <si>
+    <t>1 hrs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,8 +719,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -793,6 +807,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -1142,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1199,9 +1219,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1252,6 +1269,75 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1261,6 +1347,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1318,142 +1455,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1468,38 +1500,23 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1988,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3AB0E4-1394-414E-89C4-E0E3FFEFD8D1}">
-  <dimension ref="A2:G60"/>
+  <dimension ref="A2:G62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2027,301 +2044,301 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="65" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="85">
         <v>4</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="91" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
       <c r="E4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="53"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="92"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
       <c r="E5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="53"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="92"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="71"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
       <c r="E6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="53"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="92"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="71"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
       <c r="E7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="53"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="92"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="65" t="s">
+      <c r="A8" s="72"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="53"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="92"/>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="53"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="92"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="72"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="54"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="93"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43" t="s">
+      <c r="C11" s="65"/>
+      <c r="D11" s="65" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="85">
         <v>8</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="94" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="77"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
       <c r="E12" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="56"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="95"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="77"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
       <c r="E13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="47"/>
-      <c r="G13" s="56"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="95"/>
     </row>
     <row r="14" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="77"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
       <c r="E14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="56"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="95"/>
     </row>
     <row r="15" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="77"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
       <c r="E15" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="56"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="95"/>
     </row>
     <row r="16" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="77"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="65" t="s">
+      <c r="A16" s="54"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="56"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="95"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="77"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="56"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="95"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="78"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="48"/>
-      <c r="G18" s="57"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="96"/>
     </row>
     <row r="19" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="85" t="s">
+      <c r="A19" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43" t="s">
+      <c r="C19" s="65"/>
+      <c r="D19" s="65" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="85">
         <v>8</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="88" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="50"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="89"/>
     </row>
     <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="86"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
       <c r="E21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="50"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="89"/>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="86"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="65" t="s">
+      <c r="A22" s="83"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="50"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="89"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="86"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="50"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="89"/>
     </row>
     <row r="24" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="86"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
       <c r="E24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="50"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="89"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="87"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="48"/>
-      <c r="G25" s="51"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="90"/>
     </row>
     <row r="26" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="108" t="s">
+      <c r="B26" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="65" t="s">
         <v>46</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="46">
+      <c r="F26" s="85">
         <v>8</v>
       </c>
       <c r="G26" s="10" t="s">
@@ -2329,225 +2346,225 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="97"/>
-      <c r="B27" s="109"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
       <c r="E27" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="47"/>
+      <c r="F27" s="86"/>
       <c r="G27" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
-      <c r="B28" s="109"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="65" t="s">
+      <c r="A28" s="48"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="47"/>
+      <c r="F28" s="86"/>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="97"/>
-      <c r="B29" s="109"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="47"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="86"/>
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="97"/>
-      <c r="B30" s="109"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="65" t="s">
+      <c r="A30" s="48"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="F30" s="47"/>
+      <c r="F30" s="86"/>
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="97"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="47"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="86"/>
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="98"/>
-      <c r="B32" s="110"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
       <c r="E32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="87"/>
       <c r="G32" s="12"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="99" t="s">
+      <c r="A33" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43" t="s">
+      <c r="C33" s="65"/>
+      <c r="D33" s="65" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F33" s="46">
+      <c r="F33" s="85">
         <v>8</v>
       </c>
-      <c r="G33" s="49" t="s">
+      <c r="G33" s="88" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="100"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F34" s="47"/>
-      <c r="G34" s="50"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="89"/>
     </row>
     <row r="35" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="100"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
+      <c r="A35" s="51"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
       <c r="E35" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="50"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="89"/>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="100"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="65" t="s">
+      <c r="A36" s="51"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="47"/>
-      <c r="G36" s="50"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="89"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="50"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="89"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="101"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
       <c r="E38" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="48"/>
-      <c r="G38" s="51"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="90"/>
     </row>
     <row r="39" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43" t="s">
+      <c r="C39" s="65"/>
+      <c r="D39" s="65" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="46">
+      <c r="F39" s="85">
         <v>6</v>
       </c>
-      <c r="G39" s="49" t="s">
+      <c r="G39" s="88" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="77"/>
-      <c r="B40" s="88"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
+      <c r="A40" s="54"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
       <c r="E40" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="47"/>
-      <c r="G40" s="50"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="89"/>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="77"/>
-      <c r="B41" s="88"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="65" t="s">
+      <c r="A41" s="54"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F41" s="47"/>
-      <c r="G41" s="50"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="89"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="77"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="50"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="89"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="77"/>
-      <c r="B43" s="88"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="65" t="s">
+      <c r="A43" s="54"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="F43" s="47"/>
-      <c r="G43" s="50"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="89"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="77"/>
-      <c r="B44" s="88"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="50"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="89"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="78"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
+      <c r="A45" s="55"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
       <c r="E45" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="48"/>
-      <c r="G45" s="51"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="90"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
@@ -2556,19 +2573,19 @@
       <c r="B46" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="58" t="s">
+      <c r="C46" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="58" t="s">
+      <c r="D46" s="97" t="s">
         <v>17</v>
       </c>
       <c r="E46" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F46" s="60">
+      <c r="F46" s="99">
         <v>6</v>
       </c>
-      <c r="G46" s="62" t="s">
+      <c r="G46" s="101" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2576,241 +2593,206 @@
       <c r="A47" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
       <c r="E47" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="47"/>
-      <c r="G47" s="63"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="102"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="119" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
+      <c r="C48" s="98"/>
+      <c r="D48" s="98"/>
       <c r="E48" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F48" s="61"/>
-      <c r="G48" s="64"/>
+      <c r="F48" s="100"/>
+      <c r="G48" s="103"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="102" t="s">
+      <c r="A49" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="90" t="s">
+      <c r="B49" s="120" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43" t="s">
+      <c r="C49" s="65"/>
+      <c r="D49" s="65" t="s">
         <v>22</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F49" s="46">
+      <c r="F49" s="85">
         <v>4</v>
       </c>
-      <c r="G49" s="49" t="s">
+      <c r="G49" s="88" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="103"/>
-      <c r="B50" s="91"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
+      <c r="A50" s="57"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="66"/>
       <c r="E50" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F50" s="47"/>
-      <c r="G50" s="50"/>
+      <c r="F50" s="86"/>
+      <c r="G50" s="89"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="103"/>
-      <c r="B51" s="91"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
+      <c r="A51" s="57"/>
+      <c r="B51" s="121"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="66"/>
       <c r="E51" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F51" s="47"/>
-      <c r="G51" s="50"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="89"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="103"/>
-      <c r="B52" s="91"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="121"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
       <c r="E52" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F52" s="47"/>
-      <c r="G52" s="50"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="89"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="103"/>
-      <c r="B53" s="91"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
+      <c r="A53" s="57"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
       <c r="E53" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F53" s="47"/>
-      <c r="G53" s="50"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="89"/>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="104"/>
-      <c r="B54" s="92"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
+      <c r="A54" s="58"/>
+      <c r="B54" s="122"/>
+      <c r="C54" s="67"/>
+      <c r="D54" s="67"/>
       <c r="E54" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F54" s="48"/>
-      <c r="G54" s="51"/>
+      <c r="F54" s="87"/>
+      <c r="G54" s="90"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="105" t="s">
+      <c r="A55" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="93" t="s">
+      <c r="B55" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43" t="s">
+      <c r="C55" s="65"/>
+      <c r="D55" s="65" t="s">
         <v>30</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F55" s="46">
+      <c r="F55" s="85">
         <v>4</v>
       </c>
-      <c r="G55" s="49" t="s">
+      <c r="G55" s="88" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="106"/>
-      <c r="B56" s="94"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
+      <c r="A56" s="60"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
       <c r="E56" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="50"/>
+      <c r="F56" s="86"/>
+      <c r="G56" s="89"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="106"/>
-      <c r="B57" s="94"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="121"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="66"/>
       <c r="E57" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F57" s="47"/>
-      <c r="G57" s="50"/>
+      <c r="F57" s="86"/>
+      <c r="G57" s="89"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="106"/>
-      <c r="B58" s="94"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
+      <c r="A58" s="60"/>
+      <c r="B58" s="121"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
       <c r="E58" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F58" s="47"/>
-      <c r="G58" s="50"/>
+      <c r="F58" s="86"/>
+      <c r="G58" s="89"/>
     </row>
     <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="107"/>
-      <c r="B59" s="95"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
+      <c r="A59" s="61"/>
+      <c r="B59" s="122"/>
+      <c r="C59" s="67"/>
+      <c r="D59" s="67"/>
       <c r="E59" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F59" s="48"/>
-      <c r="G59" s="51"/>
+      <c r="F59" s="87"/>
+      <c r="G59" s="90"/>
     </row>
     <row r="60" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="123" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D60" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E60" s="22" t="s">
+      <c r="E60" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="F60" s="23">
+      <c r="F60" s="22">
         <v>8</v>
       </c>
-      <c r="G60" s="24" t="s">
+      <c r="G60" s="23" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" s="124" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C11:C18"/>
-    <mergeCell ref="D11:D18"/>
-    <mergeCell ref="D19:D25"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="B11:B18"/>
-    <mergeCell ref="C19:C25"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="F19:F25"/>
-    <mergeCell ref="G19:G25"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="D26:D32"/>
-    <mergeCell ref="F26:F32"/>
-    <mergeCell ref="F49:F54"/>
-    <mergeCell ref="G49:G54"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="F33:F38"/>
-    <mergeCell ref="G33:G38"/>
-    <mergeCell ref="C39:C45"/>
-    <mergeCell ref="D39:D45"/>
-    <mergeCell ref="F39:F45"/>
-    <mergeCell ref="G39:G45"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="E43:E44"/>
     <mergeCell ref="C55:C59"/>
     <mergeCell ref="D55:D59"/>
     <mergeCell ref="F55:F59"/>
@@ -2827,6 +2809,49 @@
     <mergeCell ref="G46:G48"/>
     <mergeCell ref="C49:C54"/>
     <mergeCell ref="D49:D54"/>
+    <mergeCell ref="F49:F54"/>
+    <mergeCell ref="G49:G54"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="F33:F38"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="D39:D45"/>
+    <mergeCell ref="F39:F45"/>
+    <mergeCell ref="G39:G45"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F19:F25"/>
+    <mergeCell ref="G19:G25"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="D26:D32"/>
+    <mergeCell ref="F26:F32"/>
+    <mergeCell ref="C11:C18"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="D19:D25"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="B11:B18"/>
+    <mergeCell ref="C19:C25"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2836,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89258D40-7AE5-4450-99B8-E9DF23DBBE8E}">
   <dimension ref="A1:G211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
@@ -2858,1816 +2883,1837 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="119">
+      <c r="A3" s="108">
         <v>1</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="112" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="33">
         <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="35" t="s">
+      <c r="A4" s="109"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="120"/>
-      <c r="B5" s="116"/>
-      <c r="C5" s="124"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="35" t="s">
+      <c r="A5" s="109"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="116"/>
-      <c r="C6" s="124"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="41" t="s">
+      <c r="A6" s="109"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="120"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="124"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="36"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="105"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="120"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="42" t="s">
+      <c r="A8" s="109"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="116"/>
-      <c r="C9" s="124"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="36"/>
+      <c r="A9" s="109"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="35"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="117"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="39" t="s">
+      <c r="A10" s="109"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="40"/>
+      <c r="G10" s="39"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
-      <c r="B11" s="115" t="s">
+      <c r="A11" s="109"/>
+      <c r="B11" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="112" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="36"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="120"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="124"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="A12" s="109"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="34"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="120"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="124"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="35" t="s">
+      <c r="A13" s="109"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="120"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="124"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="26" t="s">
+      <c r="A14" s="109"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="120"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="26" t="s">
+      <c r="A15" s="109"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="120"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="124"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="36"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="120"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="124"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="39" t="s">
+      <c r="A17" s="109"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="G17" s="40"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="120"/>
-      <c r="B18" s="115" t="s">
+      <c r="A18" s="109"/>
+      <c r="B18" s="104" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="120"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="118"/>
-      <c r="G19" s="36"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="107"/>
+      <c r="G19" s="35"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="120"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="118"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="107"/>
       <c r="E20" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="G20" s="36">
+      <c r="G20" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="120"/>
-      <c r="B21" s="116"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="118"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="36"/>
+      <c r="A21" s="109"/>
+      <c r="B21" s="105"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="107"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="120"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="118"/>
-      <c r="F22" s="26" t="s">
+      <c r="A22" s="109"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="107"/>
+      <c r="F22" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="36">
+      <c r="G22" s="35">
         <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="120"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="118"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="36"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="107"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="120"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="118"/>
-      <c r="F24" s="26" t="s">
+      <c r="A24" s="109"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="107"/>
+      <c r="F24" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="36">
+      <c r="G24" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="120"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="118"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="36"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="107"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="120"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="118"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="36"/>
+      <c r="A26" s="109"/>
+      <c r="B26" s="105"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="107"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="120"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="118"/>
-      <c r="G27" s="36"/>
+      <c r="A27" s="109"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="107"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="120"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="118"/>
-      <c r="G28" s="36"/>
+      <c r="A28" s="109"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="107"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="120"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="118"/>
-      <c r="F29" s="26" t="s">
+      <c r="A29" s="109"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="107"/>
+      <c r="F29" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G29" s="36"/>
+      <c r="G29" s="35"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="120"/>
-      <c r="B30" s="117"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="40"/>
+      <c r="A30" s="109"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="120"/>
-      <c r="B31" s="115" t="s">
+      <c r="A31" s="109"/>
+      <c r="B31" s="104" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="115" t="s">
+      <c r="C31" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="D31" s="59" t="s">
+      <c r="D31" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="120"/>
-      <c r="B32" s="116"/>
-      <c r="C32" s="116"/>
-      <c r="D32" s="118"/>
-      <c r="E32" s="35"/>
-      <c r="G32" s="36"/>
+      <c r="A32" s="109"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="34"/>
+      <c r="G32" s="35"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="120"/>
-      <c r="B33" s="116"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="35" t="s">
+      <c r="A33" s="109"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="G33" s="36">
+      <c r="G33" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="120"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="116"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="36"/>
+      <c r="A34" s="109"/>
+      <c r="B34" s="105"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="35"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="120"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="116"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="26" t="s">
+      <c r="A35" s="109"/>
+      <c r="B35" s="105"/>
+      <c r="C35" s="105"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="G35" s="36">
+      <c r="G35" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="120"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="116"/>
-      <c r="D36" s="118"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="36"/>
+      <c r="A36" s="109"/>
+      <c r="B36" s="105"/>
+      <c r="C36" s="105"/>
+      <c r="D36" s="107"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="35"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="120"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="116"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="35" t="s">
+      <c r="A37" s="109"/>
+      <c r="B37" s="105"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G37" s="36">
+      <c r="G37" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="120"/>
-      <c r="B38" s="116"/>
-      <c r="C38" s="116"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="36"/>
+      <c r="A38" s="109"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="107"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="35"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="120"/>
-      <c r="B39" s="116"/>
-      <c r="C39" s="116"/>
-      <c r="D39" s="118"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="26" t="s">
+      <c r="A39" s="109"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="105"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G39" s="36">
+      <c r="G39" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="120"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="116"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="35"/>
-      <c r="G40" s="36"/>
+      <c r="A40" s="109"/>
+      <c r="B40" s="105"/>
+      <c r="C40" s="105"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="34"/>
+      <c r="G40" s="35"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="120"/>
-      <c r="B41" s="116"/>
-      <c r="C41" s="116"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="26" t="s">
+      <c r="A41" s="109"/>
+      <c r="B41" s="105"/>
+      <c r="C41" s="105"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G41" s="36"/>
+      <c r="G41" s="35"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="120"/>
-      <c r="B42" s="117"/>
-      <c r="C42" s="117"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="40"/>
+      <c r="A42" s="109"/>
+      <c r="B42" s="106"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="97"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="39"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="120"/>
-      <c r="B43" s="115" t="s">
+      <c r="A43" s="109"/>
+      <c r="B43" s="104" t="s">
         <v>134</v>
       </c>
-      <c r="C43" s="115" t="s">
+      <c r="C43" s="104" t="s">
         <v>140</v>
       </c>
-      <c r="D43" s="59" t="s">
+      <c r="D43" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="33"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="120"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="116"/>
-      <c r="D44" s="118"/>
-      <c r="E44" s="35"/>
-      <c r="G44" s="36"/>
+      <c r="A44" s="109"/>
+      <c r="B44" s="105"/>
+      <c r="C44" s="105"/>
+      <c r="D44" s="107"/>
+      <c r="E44" s="34"/>
+      <c r="G44" s="35"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="120"/>
-      <c r="B45" s="116"/>
-      <c r="C45" s="116"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="35" t="s">
+      <c r="A45" s="109"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="105"/>
+      <c r="D45" s="107"/>
+      <c r="E45" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="F45" s="26" t="s">
+      <c r="F45" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="G45" s="36">
+      <c r="G45" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="120"/>
-      <c r="B46" s="116"/>
-      <c r="C46" s="116"/>
-      <c r="D46" s="118"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="26" t="s">
+      <c r="A46" s="109"/>
+      <c r="B46" s="105"/>
+      <c r="C46" s="105"/>
+      <c r="D46" s="107"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="G46" s="36">
+      <c r="G46" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="120"/>
-      <c r="B47" s="116"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="118"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="36"/>
+      <c r="A47" s="109"/>
+      <c r="B47" s="105"/>
+      <c r="C47" s="105"/>
+      <c r="D47" s="107"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="35"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="120"/>
-      <c r="B48" s="116"/>
-      <c r="C48" s="116"/>
-      <c r="D48" s="118"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="26" t="s">
+      <c r="A48" s="109"/>
+      <c r="B48" s="105"/>
+      <c r="C48" s="105"/>
+      <c r="D48" s="107"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="G48" s="36">
+      <c r="G48" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="120"/>
-      <c r="B49" s="116"/>
-      <c r="C49" s="116"/>
-      <c r="D49" s="118"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="26" t="s">
+      <c r="A49" s="109"/>
+      <c r="B49" s="105"/>
+      <c r="C49" s="105"/>
+      <c r="D49" s="107"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G49" s="36">
+      <c r="G49" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="120"/>
-      <c r="B50" s="116"/>
-      <c r="C50" s="116"/>
-      <c r="D50" s="118"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="26" t="s">
+      <c r="A50" s="109"/>
+      <c r="B50" s="105"/>
+      <c r="C50" s="105"/>
+      <c r="D50" s="107"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="G50" s="36"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="120"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="116"/>
-      <c r="D51" s="118"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="26" t="s">
+      <c r="A51" s="109"/>
+      <c r="B51" s="105"/>
+      <c r="C51" s="105"/>
+      <c r="D51" s="107"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="G51" s="36">
+      <c r="G51" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="120"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="116"/>
-      <c r="D52" s="118"/>
-      <c r="E52" s="35"/>
-      <c r="G52" s="36"/>
+      <c r="A52" s="109"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="107"/>
+      <c r="E52" s="34"/>
+      <c r="G52" s="35"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="120"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="118"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="26" t="s">
+      <c r="A53" s="109"/>
+      <c r="B53" s="105"/>
+      <c r="C53" s="105"/>
+      <c r="D53" s="107"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G53" s="36"/>
+      <c r="G53" s="35"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="121"/>
-      <c r="B54" s="117"/>
-      <c r="C54" s="117"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="40"/>
+      <c r="A54" s="110"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="106"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="39"/>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="113">
+      <c r="A55" s="117">
         <v>2</v>
       </c>
-      <c r="B55" s="115" t="s">
+      <c r="B55" s="104" t="s">
         <v>139</v>
       </c>
-      <c r="C55" s="115" t="s">
+      <c r="C55" s="104" t="s">
         <v>141</v>
       </c>
-      <c r="D55" s="59" t="s">
+      <c r="D55" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="31" t="s">
+      <c r="E55" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="33"/>
-      <c r="G55" s="34"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="33"/>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="114"/>
-      <c r="B56" s="116"/>
-      <c r="C56" s="116"/>
-      <c r="D56" s="118"/>
-      <c r="E56" s="35"/>
-      <c r="G56" s="36"/>
+      <c r="A56" s="118"/>
+      <c r="B56" s="105"/>
+      <c r="C56" s="105"/>
+      <c r="D56" s="107"/>
+      <c r="E56" s="34"/>
+      <c r="G56" s="35"/>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="114"/>
-      <c r="B57" s="116"/>
-      <c r="C57" s="116"/>
-      <c r="D57" s="118"/>
-      <c r="E57" s="35" t="s">
+      <c r="A57" s="118"/>
+      <c r="B57" s="105"/>
+      <c r="C57" s="105"/>
+      <c r="D57" s="107"/>
+      <c r="E57" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="F57" s="26" t="s">
+      <c r="F57" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="G57" s="36">
+      <c r="G57" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="114"/>
-      <c r="B58" s="116"/>
-      <c r="C58" s="116"/>
-      <c r="D58" s="118"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="26" t="s">
+      <c r="A58" s="118"/>
+      <c r="B58" s="105"/>
+      <c r="C58" s="105"/>
+      <c r="D58" s="107"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="G58" s="36">
+      <c r="G58" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="114"/>
-      <c r="B59" s="116"/>
-      <c r="C59" s="116"/>
-      <c r="D59" s="118"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="26" t="s">
+      <c r="A59" s="118"/>
+      <c r="B59" s="105"/>
+      <c r="C59" s="105"/>
+      <c r="D59" s="107"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="G59" s="36"/>
+      <c r="G59" s="35"/>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="114"/>
-      <c r="B60" s="116"/>
-      <c r="C60" s="116"/>
-      <c r="D60" s="118"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="26" t="s">
+      <c r="A60" s="118"/>
+      <c r="B60" s="105"/>
+      <c r="C60" s="105"/>
+      <c r="D60" s="107"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="G60" s="36">
+      <c r="G60" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="114"/>
-      <c r="B61" s="116"/>
-      <c r="C61" s="116"/>
-      <c r="D61" s="118"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="26" t="s">
+      <c r="A61" s="118"/>
+      <c r="B61" s="105"/>
+      <c r="C61" s="105"/>
+      <c r="D61" s="107"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="G61" s="36">
+      <c r="G61" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="114"/>
-      <c r="B62" s="116"/>
-      <c r="C62" s="116"/>
-      <c r="D62" s="118"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="26" t="s">
+      <c r="A62" s="118"/>
+      <c r="B62" s="105"/>
+      <c r="C62" s="105"/>
+      <c r="D62" s="107"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="G62" s="36">
+      <c r="G62" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="114"/>
-      <c r="B63" s="116"/>
-      <c r="C63" s="116"/>
-      <c r="D63" s="118"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="26" t="s">
+      <c r="A63" s="118"/>
+      <c r="B63" s="105"/>
+      <c r="C63" s="105"/>
+      <c r="D63" s="107"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="G63" s="36">
+      <c r="G63" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="114"/>
-      <c r="B64" s="116"/>
-      <c r="C64" s="116"/>
-      <c r="D64" s="118"/>
-      <c r="E64" s="35"/>
-      <c r="G64" s="36"/>
+      <c r="A64" s="118"/>
+      <c r="B64" s="105"/>
+      <c r="C64" s="105"/>
+      <c r="D64" s="107"/>
+      <c r="E64" s="34"/>
+      <c r="G64" s="35"/>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="114"/>
-      <c r="B65" s="116"/>
-      <c r="C65" s="116"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="26" t="s">
+      <c r="A65" s="118"/>
+      <c r="B65" s="105"/>
+      <c r="C65" s="105"/>
+      <c r="D65" s="107"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G65" s="36"/>
+      <c r="G65" s="35"/>
     </row>
     <row r="66" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="114"/>
-      <c r="B66" s="117"/>
-      <c r="C66" s="117"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="40"/>
+      <c r="A66" s="118"/>
+      <c r="B66" s="106"/>
+      <c r="C66" s="106"/>
+      <c r="D66" s="97"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="39"/>
     </row>
     <row r="67" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="114"/>
-      <c r="B67" s="115" t="s">
+      <c r="A67" s="118"/>
+      <c r="B67" s="104" t="s">
         <v>151</v>
       </c>
-      <c r="C67" s="115" t="s">
+      <c r="C67" s="104" t="s">
         <v>183</v>
       </c>
-      <c r="D67" s="59" t="s">
+      <c r="D67" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E67" s="31" t="s">
+      <c r="E67" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F67" s="33"/>
-      <c r="G67" s="34"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="33"/>
     </row>
     <row r="68" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="114"/>
-      <c r="B68" s="116"/>
-      <c r="C68" s="116"/>
-      <c r="D68" s="118"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="26" t="s">
+      <c r="A68" s="118"/>
+      <c r="B68" s="105"/>
+      <c r="C68" s="105"/>
+      <c r="D68" s="107"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="G68" s="36">
+      <c r="G68" s="35">
         <v>0.75</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="114"/>
-      <c r="B69" s="116"/>
-      <c r="C69" s="116"/>
-      <c r="D69" s="118"/>
-      <c r="E69" s="35" t="s">
+      <c r="A69" s="118"/>
+      <c r="B69" s="105"/>
+      <c r="C69" s="105"/>
+      <c r="D69" s="107"/>
+      <c r="E69" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="F69" s="26" t="s">
+      <c r="F69" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="G69" s="36">
+      <c r="G69" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="114"/>
-      <c r="B70" s="116"/>
-      <c r="C70" s="116"/>
-      <c r="D70" s="118"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="26" t="s">
+      <c r="A70" s="118"/>
+      <c r="B70" s="105"/>
+      <c r="C70" s="105"/>
+      <c r="D70" s="107"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="G70" s="36">
+      <c r="G70" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="114"/>
-      <c r="B71" s="116"/>
-      <c r="C71" s="116"/>
-      <c r="D71" s="118"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="26" t="s">
+      <c r="A71" s="118"/>
+      <c r="B71" s="105"/>
+      <c r="C71" s="105"/>
+      <c r="D71" s="107"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="G71" s="36">
+      <c r="G71" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="114"/>
-      <c r="B72" s="116"/>
-      <c r="C72" s="116"/>
-      <c r="D72" s="118"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="26" t="s">
+      <c r="A72" s="118"/>
+      <c r="B72" s="105"/>
+      <c r="C72" s="105"/>
+      <c r="D72" s="107"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="G72" s="36">
+      <c r="G72" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="114"/>
-      <c r="B73" s="116"/>
-      <c r="C73" s="116"/>
-      <c r="D73" s="118"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="26"/>
-      <c r="G73" s="36"/>
+      <c r="A73" s="118"/>
+      <c r="B73" s="105"/>
+      <c r="C73" s="105"/>
+      <c r="D73" s="107"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="35"/>
     </row>
     <row r="74" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="114"/>
-      <c r="B74" s="116"/>
-      <c r="C74" s="116"/>
-      <c r="D74" s="118"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="36"/>
+      <c r="A74" s="118"/>
+      <c r="B74" s="105"/>
+      <c r="C74" s="105"/>
+      <c r="D74" s="107"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="35"/>
     </row>
     <row r="75" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="114"/>
-      <c r="B75" s="116"/>
-      <c r="C75" s="116"/>
-      <c r="D75" s="118"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="26" t="s">
+      <c r="A75" s="118"/>
+      <c r="B75" s="105"/>
+      <c r="C75" s="105"/>
+      <c r="D75" s="107"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="G75" s="36">
+      <c r="G75" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="114"/>
-      <c r="B76" s="116"/>
-      <c r="C76" s="116"/>
-      <c r="D76" s="118"/>
-      <c r="E76" s="35"/>
-      <c r="G76" s="36"/>
+      <c r="A76" s="118"/>
+      <c r="B76" s="105"/>
+      <c r="C76" s="105"/>
+      <c r="D76" s="107"/>
+      <c r="E76" s="34"/>
+      <c r="G76" s="35"/>
     </row>
     <row r="77" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="114"/>
-      <c r="B77" s="116"/>
-      <c r="C77" s="116"/>
-      <c r="D77" s="118"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="26" t="s">
+      <c r="A77" s="118"/>
+      <c r="B77" s="105"/>
+      <c r="C77" s="105"/>
+      <c r="D77" s="107"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G77" s="36"/>
+      <c r="G77" s="35"/>
     </row>
     <row r="78" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="114"/>
-      <c r="B78" s="117"/>
-      <c r="C78" s="117"/>
-      <c r="D78" s="58"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="38"/>
-      <c r="G78" s="40"/>
+      <c r="A78" s="118"/>
+      <c r="B78" s="106"/>
+      <c r="C78" s="106"/>
+      <c r="D78" s="97"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="39"/>
     </row>
     <row r="79" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="114"/>
-      <c r="B79" s="115" t="s">
+      <c r="A79" s="118"/>
+      <c r="B79" s="104" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="115" t="s">
+      <c r="C79" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="D79" s="59" t="s">
+      <c r="D79" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E79" s="31" t="s">
+      <c r="E79" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F79" s="33"/>
-      <c r="G79" s="34"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="33"/>
     </row>
     <row r="80" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="114"/>
-      <c r="B80" s="116"/>
-      <c r="C80" s="116"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="35"/>
-      <c r="G80" s="36"/>
+      <c r="A80" s="118"/>
+      <c r="B80" s="105"/>
+      <c r="C80" s="105"/>
+      <c r="D80" s="107"/>
+      <c r="E80" s="34"/>
+      <c r="G80" s="35"/>
     </row>
     <row r="81" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="114"/>
-      <c r="B81" s="116"/>
-      <c r="C81" s="116"/>
-      <c r="D81" s="118"/>
-      <c r="E81" s="35" t="s">
+      <c r="A81" s="118"/>
+      <c r="B81" s="105"/>
+      <c r="C81" s="105"/>
+      <c r="D81" s="107"/>
+      <c r="E81" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="F81" s="26" t="s">
+      <c r="F81" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="G81" s="36">
+      <c r="G81" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="114"/>
-      <c r="B82" s="116"/>
-      <c r="C82" s="116"/>
-      <c r="D82" s="118"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="26" t="s">
+      <c r="A82" s="118"/>
+      <c r="B82" s="105"/>
+      <c r="C82" s="105"/>
+      <c r="D82" s="107"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="G82" s="36">
+      <c r="G82" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="114"/>
-      <c r="B83" s="116"/>
-      <c r="C83" s="116"/>
-      <c r="D83" s="118"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="26"/>
-      <c r="G83" s="36"/>
+      <c r="A83" s="118"/>
+      <c r="B83" s="105"/>
+      <c r="C83" s="105"/>
+      <c r="D83" s="107"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="35"/>
     </row>
     <row r="84" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="114"/>
-      <c r="B84" s="116"/>
-      <c r="C84" s="116"/>
-      <c r="D84" s="118"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="26" t="s">
+      <c r="A84" s="118"/>
+      <c r="B84" s="105"/>
+      <c r="C84" s="105"/>
+      <c r="D84" s="107"/>
+      <c r="E84" s="34"/>
+      <c r="F84" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="G84" s="36">
+      <c r="G84" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="114"/>
-      <c r="B85" s="116"/>
-      <c r="C85" s="116"/>
-      <c r="D85" s="118"/>
-      <c r="E85" s="35"/>
-      <c r="F85" s="26" t="s">
+      <c r="A85" s="118"/>
+      <c r="B85" s="105"/>
+      <c r="C85" s="105"/>
+      <c r="D85" s="107"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="G85" s="36">
+      <c r="G85" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="114"/>
-      <c r="B86" s="116"/>
-      <c r="C86" s="116"/>
-      <c r="D86" s="118"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="26"/>
-      <c r="G86" s="36"/>
+      <c r="A86" s="118"/>
+      <c r="B86" s="105"/>
+      <c r="C86" s="105"/>
+      <c r="D86" s="107"/>
+      <c r="E86" s="34"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="35"/>
     </row>
     <row r="87" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="114"/>
-      <c r="B87" s="116"/>
-      <c r="C87" s="116"/>
-      <c r="D87" s="118"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="26" t="s">
+      <c r="A87" s="118"/>
+      <c r="B87" s="105"/>
+      <c r="C87" s="105"/>
+      <c r="D87" s="107"/>
+      <c r="E87" s="34"/>
+      <c r="F87" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G87" s="36">
+      <c r="G87" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="114"/>
-      <c r="B88" s="116"/>
-      <c r="C88" s="116"/>
-      <c r="D88" s="118"/>
-      <c r="E88" s="35"/>
-      <c r="G88" s="36"/>
+      <c r="A88" s="118"/>
+      <c r="B88" s="105"/>
+      <c r="C88" s="105"/>
+      <c r="D88" s="107"/>
+      <c r="E88" s="34"/>
+      <c r="G88" s="35"/>
     </row>
     <row r="89" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="114"/>
-      <c r="B89" s="116"/>
-      <c r="C89" s="116"/>
-      <c r="D89" s="118"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="26" t="s">
+      <c r="A89" s="118"/>
+      <c r="B89" s="105"/>
+      <c r="C89" s="105"/>
+      <c r="D89" s="107"/>
+      <c r="E89" s="34"/>
+      <c r="F89" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G89" s="36"/>
+      <c r="G89" s="35"/>
     </row>
     <row r="90" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="114"/>
-      <c r="B90" s="117"/>
-      <c r="C90" s="117"/>
-      <c r="D90" s="58"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="40"/>
+      <c r="A90" s="118"/>
+      <c r="B90" s="106"/>
+      <c r="C90" s="106"/>
+      <c r="D90" s="97"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="39"/>
     </row>
     <row r="91" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="114"/>
-      <c r="B91" s="115" t="s">
+      <c r="A91" s="118"/>
+      <c r="B91" s="104" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="115" t="s">
+      <c r="C91" s="104" t="s">
         <v>185</v>
       </c>
-      <c r="D91" s="59" t="s">
+      <c r="D91" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E91" s="31" t="s">
+      <c r="E91" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F91" s="33"/>
-      <c r="G91" s="34"/>
+      <c r="F91" s="32"/>
+      <c r="G91" s="33"/>
     </row>
     <row r="92" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="114"/>
-      <c r="B92" s="116"/>
-      <c r="C92" s="116"/>
-      <c r="D92" s="118"/>
-      <c r="E92" s="35"/>
-      <c r="G92" s="36"/>
+      <c r="A92" s="118"/>
+      <c r="B92" s="105"/>
+      <c r="C92" s="105"/>
+      <c r="D92" s="107"/>
+      <c r="E92" s="34"/>
+      <c r="G92" s="35"/>
     </row>
     <row r="93" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="114"/>
-      <c r="B93" s="116"/>
-      <c r="C93" s="116"/>
-      <c r="D93" s="118"/>
-      <c r="E93" s="35" t="s">
+      <c r="A93" s="118"/>
+      <c r="B93" s="105"/>
+      <c r="C93" s="105"/>
+      <c r="D93" s="107"/>
+      <c r="E93" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="F93" s="26" t="s">
+      <c r="F93" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="G93" s="36">
+      <c r="G93" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="114"/>
-      <c r="B94" s="116"/>
-      <c r="C94" s="116"/>
-      <c r="D94" s="118"/>
-      <c r="E94" s="35"/>
-      <c r="F94" s="26" t="s">
+      <c r="A94" s="118"/>
+      <c r="B94" s="105"/>
+      <c r="C94" s="105"/>
+      <c r="D94" s="107"/>
+      <c r="E94" s="34"/>
+      <c r="F94" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="G94" s="36">
+      <c r="G94" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="114"/>
-      <c r="B95" s="116"/>
-      <c r="C95" s="116"/>
-      <c r="D95" s="118"/>
-      <c r="E95" s="35"/>
-      <c r="F95" s="26" t="s">
+      <c r="A95" s="118"/>
+      <c r="B95" s="105"/>
+      <c r="C95" s="105"/>
+      <c r="D95" s="107"/>
+      <c r="E95" s="34"/>
+      <c r="F95" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="G95" s="36">
+      <c r="G95" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="114"/>
-      <c r="B96" s="116"/>
-      <c r="C96" s="116"/>
-      <c r="D96" s="118"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="26" t="s">
+      <c r="A96" s="118"/>
+      <c r="B96" s="105"/>
+      <c r="C96" s="105"/>
+      <c r="D96" s="107"/>
+      <c r="E96" s="34"/>
+      <c r="F96" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="G96" s="36">
+      <c r="G96" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="114"/>
-      <c r="B97" s="116"/>
-      <c r="C97" s="116"/>
-      <c r="D97" s="118"/>
-      <c r="E97" s="35"/>
-      <c r="F97" s="26" t="s">
+      <c r="A97" s="118"/>
+      <c r="B97" s="105"/>
+      <c r="C97" s="105"/>
+      <c r="D97" s="107"/>
+      <c r="E97" s="34"/>
+      <c r="F97" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="G97" s="36">
+      <c r="G97" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="114"/>
-      <c r="B98" s="116"/>
-      <c r="C98" s="116"/>
-      <c r="D98" s="118"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="26" t="s">
+      <c r="A98" s="118"/>
+      <c r="B98" s="105"/>
+      <c r="C98" s="105"/>
+      <c r="D98" s="107"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="G98" s="36"/>
+      <c r="G98" s="35"/>
     </row>
     <row r="99" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="114"/>
-      <c r="B99" s="116"/>
-      <c r="C99" s="116"/>
-      <c r="D99" s="118"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="26"/>
-      <c r="G99" s="36"/>
+      <c r="A99" s="118"/>
+      <c r="B99" s="105"/>
+      <c r="C99" s="105"/>
+      <c r="D99" s="107"/>
+      <c r="E99" s="34"/>
+      <c r="F99" s="25"/>
+      <c r="G99" s="35"/>
     </row>
     <row r="100" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="114"/>
-      <c r="B100" s="116"/>
-      <c r="C100" s="116"/>
-      <c r="D100" s="118"/>
-      <c r="E100" s="35"/>
-      <c r="F100" s="26"/>
-      <c r="G100" s="36"/>
+      <c r="A100" s="118"/>
+      <c r="B100" s="105"/>
+      <c r="C100" s="105"/>
+      <c r="D100" s="107"/>
+      <c r="E100" s="34"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="35"/>
     </row>
     <row r="101" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="114"/>
-      <c r="B101" s="116"/>
-      <c r="C101" s="116"/>
-      <c r="D101" s="118"/>
-      <c r="E101" s="35"/>
-      <c r="F101" s="26"/>
-      <c r="G101" s="36"/>
+      <c r="A101" s="118"/>
+      <c r="B101" s="105"/>
+      <c r="C101" s="105"/>
+      <c r="D101" s="107"/>
+      <c r="E101" s="34"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="35"/>
     </row>
     <row r="102" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="114"/>
-      <c r="B102" s="116"/>
-      <c r="C102" s="116"/>
-      <c r="D102" s="118"/>
-      <c r="E102" s="35"/>
-      <c r="F102" s="26" t="s">
+      <c r="A102" s="118"/>
+      <c r="B102" s="105"/>
+      <c r="C102" s="105"/>
+      <c r="D102" s="107"/>
+      <c r="E102" s="34"/>
+      <c r="F102" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G102" s="36">
+      <c r="G102" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="114"/>
-      <c r="B103" s="116"/>
-      <c r="C103" s="116"/>
-      <c r="D103" s="118"/>
-      <c r="E103" s="35"/>
-      <c r="G103" s="36"/>
+      <c r="A103" s="118"/>
+      <c r="B103" s="105"/>
+      <c r="C103" s="105"/>
+      <c r="D103" s="107"/>
+      <c r="E103" s="34"/>
+      <c r="G103" s="35"/>
     </row>
     <row r="104" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="114"/>
-      <c r="B104" s="116"/>
-      <c r="C104" s="116"/>
-      <c r="D104" s="118"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="26" t="s">
+      <c r="A104" s="118"/>
+      <c r="B104" s="105"/>
+      <c r="C104" s="105"/>
+      <c r="D104" s="107"/>
+      <c r="E104" s="34"/>
+      <c r="F104" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G104" s="36"/>
+      <c r="G104" s="35"/>
     </row>
     <row r="105" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="114"/>
-      <c r="B105" s="117"/>
-      <c r="C105" s="117"/>
-      <c r="D105" s="58"/>
-      <c r="E105" s="37"/>
-      <c r="F105" s="38"/>
-      <c r="G105" s="40"/>
+      <c r="A105" s="118"/>
+      <c r="B105" s="106"/>
+      <c r="C105" s="106"/>
+      <c r="D105" s="97"/>
+      <c r="E105" s="36"/>
+      <c r="F105" s="37"/>
+      <c r="G105" s="39"/>
     </row>
     <row r="106" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="114"/>
-      <c r="B106" s="115" t="s">
+      <c r="A106" s="118"/>
+      <c r="B106" s="104" t="s">
         <v>174</v>
       </c>
-      <c r="C106" s="115" t="s">
+      <c r="C106" s="104" t="s">
         <v>186</v>
       </c>
-      <c r="D106" s="59" t="s">
+      <c r="D106" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E106" s="31" t="s">
+      <c r="E106" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F106" s="33"/>
-      <c r="G106" s="34"/>
+      <c r="F106" s="32"/>
+      <c r="G106" s="33"/>
     </row>
     <row r="107" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="114"/>
-      <c r="B107" s="116"/>
-      <c r="C107" s="116"/>
-      <c r="D107" s="118"/>
-      <c r="E107" s="35"/>
-      <c r="G107" s="36"/>
+      <c r="A107" s="118"/>
+      <c r="B107" s="105"/>
+      <c r="C107" s="105"/>
+      <c r="D107" s="107"/>
+      <c r="E107" s="34"/>
+      <c r="G107" s="35"/>
     </row>
     <row r="108" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="114"/>
-      <c r="B108" s="116"/>
-      <c r="C108" s="116"/>
-      <c r="D108" s="118"/>
-      <c r="E108" s="35" t="s">
+      <c r="A108" s="118"/>
+      <c r="B108" s="105"/>
+      <c r="C108" s="105"/>
+      <c r="D108" s="107"/>
+      <c r="E108" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="F108" s="26" t="s">
+      <c r="F108" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="G108" s="36">
+      <c r="G108" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="114"/>
-      <c r="B109" s="116"/>
-      <c r="C109" s="116"/>
-      <c r="D109" s="118"/>
-      <c r="E109" s="35"/>
-      <c r="F109" s="26"/>
-      <c r="G109" s="36"/>
+      <c r="A109" s="118"/>
+      <c r="B109" s="105"/>
+      <c r="C109" s="105"/>
+      <c r="D109" s="107"/>
+      <c r="E109" s="34"/>
+      <c r="F109" s="25"/>
+      <c r="G109" s="35"/>
     </row>
     <row r="110" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="114"/>
-      <c r="B110" s="116"/>
-      <c r="C110" s="116"/>
-      <c r="D110" s="118"/>
-      <c r="E110" s="35"/>
-      <c r="F110" s="26" t="s">
+      <c r="A110" s="118"/>
+      <c r="B110" s="105"/>
+      <c r="C110" s="105"/>
+      <c r="D110" s="107"/>
+      <c r="E110" s="34"/>
+      <c r="F110" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="G110" s="36">
+      <c r="G110" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="114"/>
-      <c r="B111" s="116"/>
-      <c r="C111" s="116"/>
-      <c r="D111" s="118"/>
-      <c r="E111" s="35"/>
-      <c r="F111" s="26"/>
-      <c r="G111" s="36"/>
+      <c r="A111" s="118"/>
+      <c r="B111" s="105"/>
+      <c r="C111" s="105"/>
+      <c r="D111" s="107"/>
+      <c r="E111" s="34"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="35"/>
     </row>
     <row r="112" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="114"/>
-      <c r="B112" s="116"/>
-      <c r="C112" s="116"/>
-      <c r="D112" s="118"/>
-      <c r="E112" s="35" t="s">
+      <c r="A112" s="118"/>
+      <c r="B112" s="105"/>
+      <c r="C112" s="105"/>
+      <c r="D112" s="107"/>
+      <c r="E112" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="F112" s="26" t="s">
+      <c r="F112" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="G112" s="36">
+      <c r="G112" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="114"/>
-      <c r="B113" s="116"/>
-      <c r="C113" s="116"/>
-      <c r="D113" s="118"/>
-      <c r="E113" s="35"/>
-      <c r="G113" s="36"/>
+      <c r="A113" s="118"/>
+      <c r="B113" s="105"/>
+      <c r="C113" s="105"/>
+      <c r="D113" s="107"/>
+      <c r="E113" s="34"/>
+      <c r="G113" s="35"/>
     </row>
     <row r="114" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="114"/>
-      <c r="B114" s="116"/>
-      <c r="C114" s="116"/>
-      <c r="D114" s="118"/>
-      <c r="E114" s="35"/>
-      <c r="F114" s="26" t="s">
+      <c r="A114" s="118"/>
+      <c r="B114" s="105"/>
+      <c r="C114" s="105"/>
+      <c r="D114" s="107"/>
+      <c r="E114" s="34"/>
+      <c r="F114" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="G114" s="36">
+      <c r="G114" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="114"/>
-      <c r="B115" s="116"/>
-      <c r="C115" s="116"/>
-      <c r="D115" s="118"/>
-      <c r="E115" s="35"/>
-      <c r="F115" s="26" t="s">
+      <c r="A115" s="118"/>
+      <c r="B115" s="105"/>
+      <c r="C115" s="105"/>
+      <c r="D115" s="107"/>
+      <c r="E115" s="34"/>
+      <c r="F115" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="G115" s="36">
+      <c r="G115" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="114"/>
-      <c r="B116" s="116"/>
-      <c r="C116" s="116"/>
-      <c r="D116" s="118"/>
-      <c r="E116" s="35"/>
-      <c r="F116" s="26" t="s">
+      <c r="A116" s="118"/>
+      <c r="B116" s="105"/>
+      <c r="C116" s="105"/>
+      <c r="D116" s="107"/>
+      <c r="E116" s="34"/>
+      <c r="F116" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="G116" s="36">
+      <c r="G116" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="114"/>
-      <c r="B117" s="116"/>
-      <c r="C117" s="116"/>
-      <c r="D117" s="118"/>
-      <c r="E117" s="35"/>
-      <c r="F117" s="26"/>
-      <c r="G117" s="36"/>
+      <c r="A117" s="118"/>
+      <c r="B117" s="105"/>
+      <c r="C117" s="105"/>
+      <c r="D117" s="107"/>
+      <c r="E117" s="34"/>
+      <c r="F117" s="25"/>
+      <c r="G117" s="35"/>
     </row>
     <row r="118" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="114"/>
-      <c r="B118" s="116"/>
-      <c r="C118" s="116"/>
-      <c r="D118" s="118"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="26" t="s">
+      <c r="A118" s="118"/>
+      <c r="B118" s="105"/>
+      <c r="C118" s="105"/>
+      <c r="D118" s="107"/>
+      <c r="E118" s="34"/>
+      <c r="F118" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G118" s="36">
+      <c r="G118" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="114"/>
-      <c r="B119" s="116"/>
-      <c r="C119" s="116"/>
-      <c r="D119" s="118"/>
-      <c r="E119" s="35"/>
-      <c r="G119" s="36"/>
+      <c r="A119" s="118"/>
+      <c r="B119" s="105"/>
+      <c r="C119" s="105"/>
+      <c r="D119" s="107"/>
+      <c r="E119" s="34"/>
+      <c r="G119" s="35"/>
     </row>
     <row r="120" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="114"/>
-      <c r="B120" s="116"/>
-      <c r="C120" s="116"/>
-      <c r="D120" s="118"/>
-      <c r="E120" s="35"/>
-      <c r="F120" s="26" t="s">
+      <c r="A120" s="118"/>
+      <c r="B120" s="105"/>
+      <c r="C120" s="105"/>
+      <c r="D120" s="107"/>
+      <c r="E120" s="34"/>
+      <c r="F120" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G120" s="36"/>
+      <c r="G120" s="35"/>
     </row>
     <row r="121" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="114"/>
-      <c r="B121" s="117"/>
-      <c r="C121" s="117"/>
-      <c r="D121" s="58"/>
-      <c r="E121" s="37"/>
-      <c r="F121" s="38"/>
-      <c r="G121" s="40"/>
+      <c r="A121" s="118"/>
+      <c r="B121" s="106"/>
+      <c r="C121" s="106"/>
+      <c r="D121" s="97"/>
+      <c r="E121" s="36"/>
+      <c r="F121" s="37"/>
+      <c r="G121" s="39"/>
     </row>
     <row r="122" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="111">
+      <c r="A122" s="115">
         <v>3</v>
       </c>
-      <c r="B122" s="115" t="s">
+      <c r="B122" s="104" t="s">
         <v>182</v>
       </c>
-      <c r="C122" s="115" t="s">
+      <c r="C122" s="104" t="s">
         <v>187</v>
       </c>
-      <c r="D122" s="59" t="s">
+      <c r="D122" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="E122" s="31" t="s">
+      <c r="E122" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F122" s="33"/>
-      <c r="G122" s="34"/>
+      <c r="F122" s="32"/>
+      <c r="G122" s="33"/>
     </row>
     <row r="123" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="112"/>
-      <c r="B123" s="116"/>
-      <c r="C123" s="116"/>
-      <c r="D123" s="118"/>
-      <c r="E123" s="35"/>
-      <c r="G123" s="36"/>
+      <c r="A123" s="116"/>
+      <c r="B123" s="105"/>
+      <c r="C123" s="105"/>
+      <c r="D123" s="107"/>
+      <c r="E123" s="34"/>
+      <c r="G123" s="35"/>
     </row>
     <row r="124" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="112"/>
-      <c r="B124" s="116"/>
-      <c r="C124" s="116"/>
-      <c r="D124" s="118"/>
-      <c r="E124" s="35" t="s">
+      <c r="A124" s="116"/>
+      <c r="B124" s="105"/>
+      <c r="C124" s="105"/>
+      <c r="D124" s="107"/>
+      <c r="E124" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="F124" s="26" t="s">
+      <c r="F124" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="G124" s="36">
+      <c r="G124" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="112"/>
-      <c r="B125" s="116"/>
-      <c r="C125" s="116"/>
-      <c r="D125" s="118"/>
-      <c r="E125" s="35"/>
-      <c r="F125" s="26"/>
-      <c r="G125" s="36"/>
+      <c r="A125" s="116"/>
+      <c r="B125" s="105"/>
+      <c r="C125" s="105"/>
+      <c r="D125" s="107"/>
+      <c r="E125" s="34"/>
+      <c r="F125" s="25"/>
+      <c r="G125" s="35"/>
     </row>
     <row r="126" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="112"/>
-      <c r="B126" s="116"/>
-      <c r="C126" s="116"/>
-      <c r="D126" s="118"/>
-      <c r="E126" s="35"/>
-      <c r="F126" s="26" t="s">
+      <c r="A126" s="116"/>
+      <c r="B126" s="105"/>
+      <c r="C126" s="105"/>
+      <c r="D126" s="107"/>
+      <c r="E126" s="34"/>
+      <c r="F126" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="G126" s="36">
+      <c r="G126" s="35">
         <v>0.25</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="112"/>
-      <c r="B127" s="116"/>
-      <c r="C127" s="116"/>
-      <c r="D127" s="118"/>
-      <c r="E127" s="35"/>
-      <c r="F127" s="26"/>
-      <c r="G127" s="36"/>
+      <c r="A127" s="116"/>
+      <c r="B127" s="105"/>
+      <c r="C127" s="105"/>
+      <c r="D127" s="107"/>
+      <c r="E127" s="34"/>
+      <c r="F127" s="25"/>
+      <c r="G127" s="35"/>
     </row>
     <row r="128" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="112"/>
-      <c r="B128" s="116"/>
-      <c r="C128" s="116"/>
-      <c r="D128" s="118"/>
-      <c r="E128" s="35" t="s">
+      <c r="A128" s="116"/>
+      <c r="B128" s="105"/>
+      <c r="C128" s="105"/>
+      <c r="D128" s="107"/>
+      <c r="E128" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="F128" s="26" t="s">
+      <c r="F128" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="G128" s="36">
+      <c r="G128" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="112"/>
-      <c r="B129" s="116"/>
-      <c r="C129" s="116"/>
-      <c r="D129" s="118"/>
-      <c r="E129" s="35"/>
-      <c r="G129" s="36"/>
+      <c r="A129" s="116"/>
+      <c r="B129" s="105"/>
+      <c r="C129" s="105"/>
+      <c r="D129" s="107"/>
+      <c r="E129" s="34"/>
+      <c r="G129" s="35"/>
     </row>
     <row r="130" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="112"/>
-      <c r="B130" s="116"/>
-      <c r="C130" s="116"/>
-      <c r="D130" s="118"/>
-      <c r="E130" s="35"/>
-      <c r="F130" s="26" t="s">
+      <c r="A130" s="116"/>
+      <c r="B130" s="105"/>
+      <c r="C130" s="105"/>
+      <c r="D130" s="107"/>
+      <c r="E130" s="34"/>
+      <c r="F130" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="G130" s="36">
+      <c r="G130" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="112"/>
-      <c r="B131" s="116"/>
-      <c r="C131" s="116"/>
-      <c r="D131" s="118"/>
-      <c r="E131" s="35"/>
-      <c r="F131" s="26" t="s">
+      <c r="A131" s="116"/>
+      <c r="B131" s="105"/>
+      <c r="C131" s="105"/>
+      <c r="D131" s="107"/>
+      <c r="E131" s="34"/>
+      <c r="F131" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="G131" s="36">
+      <c r="G131" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="112"/>
-      <c r="B132" s="116"/>
-      <c r="C132" s="116"/>
-      <c r="D132" s="118"/>
-      <c r="E132" s="35"/>
-      <c r="F132" s="26" t="s">
+      <c r="A132" s="116"/>
+      <c r="B132" s="105"/>
+      <c r="C132" s="105"/>
+      <c r="D132" s="107"/>
+      <c r="E132" s="34"/>
+      <c r="F132" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="G132" s="36">
+      <c r="G132" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="112"/>
-      <c r="B133" s="116"/>
-      <c r="C133" s="116"/>
-      <c r="D133" s="118"/>
-      <c r="E133" s="35"/>
-      <c r="F133" s="26"/>
-      <c r="G133" s="36"/>
+      <c r="A133" s="116"/>
+      <c r="B133" s="105"/>
+      <c r="C133" s="105"/>
+      <c r="D133" s="107"/>
+      <c r="E133" s="34"/>
+      <c r="F133" s="25"/>
+      <c r="G133" s="35"/>
     </row>
     <row r="134" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="112"/>
-      <c r="B134" s="116"/>
-      <c r="C134" s="116"/>
-      <c r="D134" s="118"/>
-      <c r="E134" s="35"/>
-      <c r="F134" s="26" t="s">
+      <c r="A134" s="116"/>
+      <c r="B134" s="105"/>
+      <c r="C134" s="105"/>
+      <c r="D134" s="107"/>
+      <c r="E134" s="34"/>
+      <c r="F134" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G134" s="36">
+      <c r="G134" s="35">
         <v>0.5</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="112"/>
-      <c r="B135" s="116"/>
-      <c r="C135" s="116"/>
-      <c r="D135" s="118"/>
-      <c r="E135" s="35"/>
-      <c r="G135" s="36"/>
+      <c r="A135" s="116"/>
+      <c r="B135" s="105"/>
+      <c r="C135" s="105"/>
+      <c r="D135" s="107"/>
+      <c r="E135" s="34"/>
+      <c r="G135" s="35"/>
     </row>
     <row r="136" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="112"/>
-      <c r="B136" s="116"/>
-      <c r="C136" s="116"/>
-      <c r="D136" s="118"/>
-      <c r="E136" s="35"/>
-      <c r="F136" s="26" t="s">
+      <c r="A136" s="116"/>
+      <c r="B136" s="105"/>
+      <c r="C136" s="105"/>
+      <c r="D136" s="107"/>
+      <c r="E136" s="34"/>
+      <c r="F136" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G136" s="36"/>
+      <c r="G136" s="35"/>
     </row>
     <row r="137" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="112"/>
-      <c r="B137" s="117"/>
-      <c r="C137" s="117"/>
-      <c r="D137" s="58"/>
-      <c r="E137" s="37"/>
-      <c r="F137" s="38"/>
-      <c r="G137" s="40"/>
+      <c r="A137" s="116"/>
+      <c r="B137" s="106"/>
+      <c r="C137" s="106"/>
+      <c r="D137" s="97"/>
+      <c r="E137" s="36"/>
+      <c r="F137" s="37"/>
+      <c r="G137" s="39"/>
     </row>
     <row r="138" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="112"/>
+      <c r="A138" s="116"/>
     </row>
     <row r="139" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="112"/>
+      <c r="A139" s="116"/>
     </row>
     <row r="140" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="112"/>
+      <c r="A140" s="116"/>
     </row>
     <row r="141" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="112"/>
+      <c r="A141" s="116"/>
     </row>
     <row r="142" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="112"/>
+      <c r="A142" s="116"/>
     </row>
     <row r="143" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="112"/>
+      <c r="A143" s="116"/>
     </row>
     <row r="144" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="112"/>
+      <c r="A144" s="116"/>
     </row>
     <row r="145" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="112"/>
+      <c r="A145" s="116"/>
     </row>
     <row r="146" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="112"/>
+      <c r="A146" s="116"/>
     </row>
     <row r="147" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="112"/>
+      <c r="A147" s="116"/>
     </row>
     <row r="148" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="112"/>
+      <c r="A148" s="116"/>
     </row>
     <row r="149" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="112"/>
+      <c r="A149" s="116"/>
     </row>
     <row r="150" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="112"/>
+      <c r="A150" s="116"/>
     </row>
     <row r="151" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="112"/>
+      <c r="A151" s="116"/>
     </row>
     <row r="152" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="112"/>
+      <c r="A152" s="116"/>
     </row>
     <row r="153" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="112"/>
+      <c r="A153" s="116"/>
     </row>
     <row r="154" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="112"/>
+      <c r="A154" s="116"/>
     </row>
     <row r="155" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="112"/>
+      <c r="A155" s="116"/>
     </row>
     <row r="156" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="112"/>
+      <c r="A156" s="116"/>
     </row>
     <row r="157" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="112"/>
+      <c r="A157" s="116"/>
     </row>
     <row r="158" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="112"/>
+      <c r="A158" s="116"/>
     </row>
     <row r="159" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="112"/>
+      <c r="A159" s="116"/>
     </row>
     <row r="160" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="112"/>
+      <c r="A160" s="116"/>
     </row>
     <row r="161" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="112"/>
+      <c r="A161" s="116"/>
     </row>
     <row r="162" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="112"/>
+      <c r="A162" s="116"/>
     </row>
     <row r="163" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="112"/>
+      <c r="A163" s="116"/>
     </row>
     <row r="164" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="112"/>
+      <c r="A164" s="116"/>
     </row>
     <row r="165" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="112"/>
+      <c r="A165" s="116"/>
     </row>
     <row r="166" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="112"/>
+      <c r="A166" s="116"/>
     </row>
     <row r="167" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="112"/>
+      <c r="A167" s="116"/>
     </row>
     <row r="168" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="112"/>
+      <c r="A168" s="116"/>
     </row>
     <row r="169" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="112"/>
+      <c r="A169" s="116"/>
     </row>
     <row r="170" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="112"/>
+      <c r="A170" s="116"/>
     </row>
     <row r="171" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="112"/>
+      <c r="A171" s="116"/>
     </row>
     <row r="172" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="112"/>
+      <c r="A172" s="116"/>
     </row>
     <row r="173" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="112"/>
+      <c r="A173" s="116"/>
     </row>
     <row r="174" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="112"/>
+      <c r="A174" s="116"/>
     </row>
     <row r="175" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="112"/>
+      <c r="A175" s="116"/>
     </row>
     <row r="176" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="112"/>
+      <c r="A176" s="116"/>
     </row>
     <row r="177" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="112"/>
+      <c r="A177" s="116"/>
     </row>
     <row r="178" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="112"/>
+      <c r="A178" s="116"/>
     </row>
     <row r="179" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="112"/>
+      <c r="A179" s="116"/>
     </row>
     <row r="180" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="112"/>
+      <c r="A180" s="116"/>
     </row>
     <row r="181" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="112"/>
+      <c r="A181" s="116"/>
     </row>
     <row r="182" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="112"/>
+      <c r="A182" s="116"/>
     </row>
     <row r="183" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="112"/>
+      <c r="A183" s="116"/>
     </row>
     <row r="184" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="112"/>
+      <c r="A184" s="116"/>
     </row>
     <row r="185" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="112"/>
+      <c r="A185" s="116"/>
     </row>
     <row r="186" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="112"/>
+      <c r="A186" s="116"/>
     </row>
     <row r="187" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="112"/>
+      <c r="A187" s="116"/>
     </row>
     <row r="188" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="112"/>
+      <c r="A188" s="116"/>
     </row>
     <row r="189" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="113"/>
+      <c r="A189" s="117"/>
     </row>
     <row r="190" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="114"/>
+      <c r="A190" s="118"/>
     </row>
     <row r="191" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="114"/>
+      <c r="A191" s="118"/>
     </row>
     <row r="192" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="114"/>
+      <c r="A192" s="118"/>
     </row>
     <row r="193" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="114"/>
+      <c r="A193" s="118"/>
     </row>
     <row r="194" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="114"/>
+      <c r="A194" s="118"/>
     </row>
     <row r="195" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="114"/>
+      <c r="A195" s="118"/>
     </row>
     <row r="196" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="114"/>
+      <c r="A196" s="118"/>
     </row>
     <row r="197" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="114"/>
+      <c r="A197" s="118"/>
     </row>
     <row r="198" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="114"/>
+      <c r="A198" s="118"/>
     </row>
     <row r="199" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="114"/>
+      <c r="A199" s="118"/>
     </row>
     <row r="200" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="114"/>
+      <c r="A200" s="118"/>
     </row>
     <row r="201" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="114"/>
+      <c r="A201" s="118"/>
     </row>
     <row r="202" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="114"/>
+      <c r="A202" s="118"/>
     </row>
     <row r="203" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="114"/>
+      <c r="A203" s="118"/>
     </row>
     <row r="204" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="114"/>
+      <c r="A204" s="118"/>
     </row>
     <row r="205" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="114"/>
+      <c r="A205" s="118"/>
     </row>
     <row r="206" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="114"/>
+      <c r="A206" s="118"/>
     </row>
     <row r="207" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="114"/>
+      <c r="A207" s="118"/>
     </row>
     <row r="208" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="114"/>
+      <c r="A208" s="118"/>
     </row>
     <row r="209" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="114"/>
+      <c r="A209" s="118"/>
     </row>
     <row r="210" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="114"/>
+      <c r="A210" s="118"/>
     </row>
     <row r="211" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="114"/>
+      <c r="A211" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A122:A188"/>
+    <mergeCell ref="A189:A211"/>
+    <mergeCell ref="B55:B66"/>
+    <mergeCell ref="C55:C66"/>
+    <mergeCell ref="D55:D66"/>
+    <mergeCell ref="B67:B78"/>
+    <mergeCell ref="C67:C78"/>
+    <mergeCell ref="D67:D78"/>
+    <mergeCell ref="A55:A121"/>
+    <mergeCell ref="B122:B137"/>
+    <mergeCell ref="C122:C137"/>
+    <mergeCell ref="D122:D137"/>
+    <mergeCell ref="B79:B90"/>
+    <mergeCell ref="C79:C90"/>
+    <mergeCell ref="D79:D90"/>
+    <mergeCell ref="B91:B105"/>
+    <mergeCell ref="C91:C105"/>
+    <mergeCell ref="D91:D105"/>
+    <mergeCell ref="B106:B121"/>
+    <mergeCell ref="C106:C121"/>
+    <mergeCell ref="D106:D121"/>
     <mergeCell ref="B18:B30"/>
     <mergeCell ref="C18:C30"/>
     <mergeCell ref="D18:D30"/>
@@ -4684,27 +4730,6 @@
     <mergeCell ref="B43:B54"/>
     <mergeCell ref="C43:C54"/>
     <mergeCell ref="D43:D54"/>
-    <mergeCell ref="C91:C105"/>
-    <mergeCell ref="D91:D105"/>
-    <mergeCell ref="B106:B121"/>
-    <mergeCell ref="C106:C121"/>
-    <mergeCell ref="D106:D121"/>
-    <mergeCell ref="A122:A188"/>
-    <mergeCell ref="A189:A211"/>
-    <mergeCell ref="B55:B66"/>
-    <mergeCell ref="C55:C66"/>
-    <mergeCell ref="D55:D66"/>
-    <mergeCell ref="B67:B78"/>
-    <mergeCell ref="C67:C78"/>
-    <mergeCell ref="D67:D78"/>
-    <mergeCell ref="A55:A121"/>
-    <mergeCell ref="B122:B137"/>
-    <mergeCell ref="C122:C137"/>
-    <mergeCell ref="D122:D137"/>
-    <mergeCell ref="B79:B90"/>
-    <mergeCell ref="C79:C90"/>
-    <mergeCell ref="D79:D90"/>
-    <mergeCell ref="B91:B105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4724,7 +4749,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L3" s="25">
+      <c r="L3" s="24">
         <v>45567</v>
       </c>
       <c r="M3" t="s">
@@ -4732,7 +4757,7 @@
       </c>
     </row>
     <row r="4" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L4" s="25">
+      <c r="L4" s="24">
         <v>45576</v>
       </c>
       <c r="M4" t="s">
@@ -4740,7 +4765,7 @@
       </c>
     </row>
     <row r="5" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L5" s="25">
+      <c r="L5" s="24">
         <v>45576</v>
       </c>
       <c r="M5" t="s">
@@ -4748,7 +4773,7 @@
       </c>
     </row>
     <row r="6" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L6" s="25">
+      <c r="L6" s="24">
         <v>45582</v>
       </c>
       <c r="M6" t="s">
@@ -4756,7 +4781,7 @@
       </c>
     </row>
     <row r="7" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L7" s="25">
+      <c r="L7" s="24">
         <v>45596</v>
       </c>
       <c r="M7" t="s">
@@ -4764,7 +4789,7 @@
       </c>
     </row>
     <row r="8" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L8" s="25">
+      <c r="L8" s="24">
         <v>45597</v>
       </c>
       <c r="M8" t="s">
@@ -4772,7 +4797,7 @@
       </c>
     </row>
     <row r="9" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L9" s="25">
+      <c r="L9" s="24">
         <v>45611</v>
       </c>
       <c r="M9" t="s">
@@ -4780,7 +4805,7 @@
       </c>
     </row>
     <row r="10" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L10" s="25">
+      <c r="L10" s="24">
         <v>45651</v>
       </c>
       <c r="M10" t="s">

</xml_diff>